<commit_message>
added logic for finding headers
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/customer.xlsx
+++ b/src/main/resources/excel/customer.xlsx
@@ -13,13 +13,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
+    <t>customer_name</t>
+  </si>
+  <si>
+    <t>customer_password</t>
+  </si>
+  <si>
     <t>customer_id</t>
-  </si>
-  <si>
-    <t>customer_name</t>
-  </si>
-  <si>
-    <t>customer_password</t>
   </si>
   <si>
     <t>shiva</t>
@@ -319,48 +319,51 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
         <v>1.0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
         <v>2.0</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
         <v>3.0</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
         <v>4.0</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>